<commit_message>
documentation update, info.txt for characteristics settings
</commit_message>
<xml_diff>
--- a/Algorithm/Characteristics_Setting/15.newMol_1/characteristics_data.xlsx
+++ b/Algorithm/Characteristics_Setting/15.newMol_1/characteristics_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Giuliana\Dropbox\Tesi\scerpa\Algorithm\Characteristics_Setting\newMol_th2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\scerpa\Algorithm\Characteristics_Setting\15.newMol_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C5F7E3B-06F8-4A6F-9BA5-AC0D48D184B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F607228-27E0-4769-8322-4D7109ED641D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7248" yWindow="2124" windowWidth="15072" windowHeight="8904" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5064" yWindow="924" windowWidth="16140" windowHeight="10128" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>File Name</t>
   </si>
@@ -36,15 +36,12 @@
   <si>
     <t>ck1.txt</t>
   </si>
-  <si>
-    <t>ck2.txt</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -52,6 +49,13 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -78,9 +82,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -356,10 +361,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -370,7 +375,7 @@
     <col min="4" max="1025" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -381,38 +386,30 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2">
         <v>-2</v>
       </c>
-      <c r="C2">
-        <v>39</v>
+      <c r="C2" s="1">
+        <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3">
-        <v>39</v>
+    <row r="3" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1">
+        <v>70</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1">
-        <v>2</v>
-      </c>
-      <c r="C4" s="1">
-        <v>70</v>
-      </c>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D5" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>